<commit_message>
fixed address truncation. added EEPROM support
</commit_message>
<xml_diff>
--- a/BootloaderCMDList.xlsx
+++ b/BootloaderCMDList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>ID</t>
   </si>
@@ -265,15 +265,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>aa aa aa aa</t>
-  </si>
-  <si>
     <t>led on</t>
   </si>
   <si>
@@ -287,6 +278,36 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>nrfTXaddr</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Read EEPROM byte</t>
+  </si>
+  <si>
+    <t>Write EEPROM byte</t>
+  </si>
+  <si>
+    <t>EEPROM erase all</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>pp bb vv</t>
+  </si>
+  <si>
+    <t>pp bb</t>
   </si>
 </sst>
 </file>
@@ -360,13 +381,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -698,17 +719,17 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
@@ -776,7 +797,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
@@ -795,7 +816,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="s">
@@ -847,7 +868,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
@@ -858,13 +879,13 @@
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
@@ -970,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G38"/>
+  <dimension ref="B2:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,16 +1007,8 @@
     <col min="7" max="7" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" t="s">
-        <v>80</v>
-      </c>
-    </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
@@ -1003,7 +1016,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
@@ -1021,9 +1034,7 @@
         <v>39</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -1035,9 +1046,7 @@
       <c r="D6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
@@ -1105,16 +1114,16 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
@@ -1125,7 +1134,7 @@
       <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1144,106 +1153,144 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>26</v>
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>28</v>
+      <c r="B22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>